<commit_message>
update out of stock update process
</commit_message>
<xml_diff>
--- a/public/uploads/out_of_stocks/out_of_stock_list_88.xlsx
+++ b/public/uploads/out_of_stocks/out_of_stock_list_88.xlsx
@@ -4,22 +4,17 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="25365" windowHeight="14595" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
   <si>
     <t>ID</t>
   </si>
@@ -45,6 +40,9 @@
     <t>Batch Number</t>
   </si>
   <si>
+    <t>Expiry Date (dd-mm-yyyy)</t>
+  </si>
+  <si>
     <t>Current Stringent Regulatory Authority (SRA) Approvals</t>
   </si>
   <si>
@@ -60,25 +58,34 @@
     <t>Average Monthly Consumption (AMC) in Packs</t>
   </si>
   <si>
-    <t>mg</t>
-  </si>
-  <si>
-    <t>Expiry Date (yyyy-mm-dd)</t>
+    <t>testing *x3</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>testing *x1</t>
+  </si>
+  <si>
+    <t>Other</t>
   </si>
   <si>
     <t>g487654</t>
   </si>
   <si>
-    <t>testing *12</t>
+    <t>test</t>
+  </si>
+  <si>
+    <t>testing *x2</t>
+  </si>
+  <si>
+    <t>15/2018</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -119,16 +126,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,21 +471,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="96" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" zoomScale="66" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
     <col min="3" max="4" width="20" customWidth="1"/>
     <col min="5" max="6" width="30" customWidth="1"/>
     <col min="7" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="30" style="3" customWidth="1"/>
-    <col min="10" max="10" width="30" customWidth="1"/>
+    <col min="9" max="10" width="30" customWidth="1"/>
     <col min="11" max="13" width="20" customWidth="1"/>
     <col min="14" max="14" width="30" customWidth="1"/>
   </cols>
@@ -512,71 +514,159 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>14</v>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
+        <v>7013</v>
+      </c>
+      <c r="B2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>16</v>
+      <c r="C2" t="s">
+        <v>17</v>
       </c>
       <c r="D2">
         <v>1000</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" t="s">
         <v>16</v>
       </c>
       <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="2">
+        <v>43451</v>
+      </c>
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2">
+        <v>1245</v>
+      </c>
+      <c r="L2">
+        <v>56</v>
+      </c>
+      <c r="M2">
+        <v>3</v>
+      </c>
+      <c r="N2" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="4">
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2345678</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3">
+        <v>1000</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3">
         <v>1245</v>
       </c>
+      <c r="L3">
+        <v>56</v>
+      </c>
+      <c r="M3">
+        <v>4</v>
+      </c>
+      <c r="N3" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>17013</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4">
+        <v>1000</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="2">
+        <v>43451</v>
+      </c>
+      <c r="J4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4">
+        <v>1245</v>
+      </c>
+      <c r="L4">
+        <v>56</v>
+      </c>
+      <c r="M4">
+        <v>3</v>
+      </c>
+      <c r="N4" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>